<commit_message>
Running code from cmd line
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRMTestData.xlsx
+++ b/TestData/OrangeHRMTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctipuran\eclipse-workspace\MavenProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F9E3B6-FCDF-4A9A-B936-C6D41C9763CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B522227A-3B3B-467F-98B9-7DBFCA946B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7270" xr2:uid="{2E5588A1-4D1B-45C4-9EF5-03800DE63DD2}"/>
   </bookViews>
@@ -61,10 +61,10 @@
     <t>Admin1</t>
   </si>
   <si>
-    <t>admin@123</t>
-  </si>
-  <si>
-    <t>Invalid</t>
+    <t>InValid</t>
+  </si>
+  <si>
+    <t>admin#123</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,11 +472,11 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -484,10 +484,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -503,7 +503,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{4087DA25-20EA-40F6-B775-0A0A55527D82}"/>
+    <hyperlink ref="B3" r:id="rId1" display="admin@123" xr:uid="{8B08B008-760B-4104-BBA8-35CE24D63F6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>